<commit_message>
Add default values for attributes
</commit_message>
<xml_diff>
--- a/docs/excel_template.xlsx
+++ b/docs/excel_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\excelPlayground\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D73E4E-0806-4DC0-8953-23C5D072C03C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522AE18B-6A20-4BF9-988C-58739E65965A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D76963E8-864B-457D-9DF5-20326BDCEA33}"/>
+    <workbookView xWindow="12600" yWindow="1640" windowWidth="19200" windowHeight="7640" activeTab="1" xr2:uid="{D76963E8-864B-457D-9DF5-20326BDCEA33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F6C0FE-C9D2-4B77-A5CF-E298AC22F6EE}">
   <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update senders and receivers to include all info from the excel template
</commit_message>
<xml_diff>
--- a/docs/excel_template.xlsx
+++ b/docs/excel_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522AE18B-6A20-4BF9-988C-58739E65965A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E27E86F-24BD-467A-B690-73E174DD25DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="1640" windowWidth="19200" windowHeight="7640" activeTab="1" xr2:uid="{D76963E8-864B-457D-9DF5-20326BDCEA33}"/>
+    <workbookView xWindow="0" yWindow="2280" windowWidth="19200" windowHeight="7640" activeTab="1" xr2:uid="{D76963E8-864B-457D-9DF5-20326BDCEA33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -660,11 +660,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F6C0FE-C9D2-4B77-A5CF-E298AC22F6EE}">
   <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29" customWidth="1"/>
+    <col min="24" max="24" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Add more styling/container ID field
</commit_message>
<xml_diff>
--- a/docs/excel_template.xlsx
+++ b/docs/excel_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E27E86F-24BD-467A-B690-73E174DD25DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54CB498-9F0A-452A-BF91-7DFA74EC0804}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2280" windowWidth="19200" windowHeight="7640" activeTab="1" xr2:uid="{D76963E8-864B-457D-9DF5-20326BDCEA33}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D76963E8-864B-457D-9DF5-20326BDCEA33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F6C0FE-C9D2-4B77-A5CF-E298AC22F6EE}">
   <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Create new excel template to match DB schema changesg
</commit_message>
<xml_diff>
--- a/docs/excel_template.xlsx
+++ b/docs/excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\Barko\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77620F89-3739-46FA-B898-A9FB16B40FD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D280CA4-24DF-41A0-B24A-637C12FEEF37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D76963E8-864B-457D-9DF5-20326BDCEA33}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Count</t>
   </si>
@@ -67,138 +67,6 @@
   </si>
   <si>
     <t>Contact Number(s)</t>
-  </si>
-  <si>
-    <t>SHIP_1</t>
-  </si>
-  <si>
-    <t>Auckland</t>
-  </si>
-  <si>
-    <t>Travolta</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
-    <t>+64226739516</t>
-  </si>
-  <si>
-    <t>Kalalo</t>
-  </si>
-  <si>
-    <t>Ivy</t>
-  </si>
-  <si>
-    <t>Medrano</t>
-  </si>
-  <si>
-    <t>2 Sunshine St</t>
-  </si>
-  <si>
-    <t>Batangas</t>
-  </si>
-  <si>
-    <t>Philippines</t>
-  </si>
-  <si>
-    <t>+639158577500</t>
-  </si>
-  <si>
-    <t>SHIP_2</t>
-  </si>
-  <si>
-    <t>Foxx</t>
-  </si>
-  <si>
-    <t>Jamie</t>
-  </si>
-  <si>
-    <t>+64211052385</t>
-  </si>
-  <si>
-    <t>Balbin</t>
-  </si>
-  <si>
-    <t>Emelva</t>
-  </si>
-  <si>
-    <t>More</t>
-  </si>
-  <si>
-    <t>48 Gemini Way</t>
-  </si>
-  <si>
-    <t>Davao</t>
-  </si>
-  <si>
-    <t>Davai</t>
-  </si>
-  <si>
-    <t>+639083842100</t>
-  </si>
-  <si>
-    <t>SHIP_3</t>
-  </si>
-  <si>
-    <t>West</t>
-  </si>
-  <si>
-    <t>Kane</t>
-  </si>
-  <si>
-    <t>Patigdas</t>
-  </si>
-  <si>
-    <t>Gladdy</t>
-  </si>
-  <si>
-    <t>59 Somserset Street</t>
-  </si>
-  <si>
-    <t>General Trias</t>
-  </si>
-  <si>
-    <t>Cavite</t>
-  </si>
-  <si>
-    <t>+639067079199</t>
-  </si>
-  <si>
-    <t>SHIP_4</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Whitney</t>
-  </si>
-  <si>
-    <t>Jackson</t>
-  </si>
-  <si>
-    <t>+64211052395</t>
-  </si>
-  <si>
-    <t>Quindo</t>
-  </si>
-  <si>
-    <t>Steve</t>
-  </si>
-  <si>
-    <t>Mamaradlo</t>
-  </si>
-  <si>
-    <t>30 Bagus Way</t>
-  </si>
-  <si>
-    <t>+639083932100</t>
   </si>
 </sst>
 </file>
@@ -255,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -272,11 +140,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -291,6 +168,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,7 +487,7 @@
   <dimension ref="A1:Q140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -686,212 +565,80 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>35</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2" s="12"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="13"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2" s="11"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3" s="13"/>
+      <c r="E3"/>
       <c r="F3"/>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>36</v>
-      </c>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="13"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3" s="11"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4" s="13"/>
+      <c r="E4"/>
       <c r="F4"/>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" t="s">
-        <v>43</v>
-      </c>
-      <c r="O4" t="s">
-        <v>44</v>
-      </c>
-      <c r="P4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>45</v>
-      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="13"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" t="s">
-        <v>54</v>
-      </c>
-      <c r="N5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>55</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5" s="13"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="13"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>

</xml_diff>